<commit_message>
Excel tables added to uploadExcel folder
</commit_message>
<xml_diff>
--- a/back-end/uploadExcel/faculty_qualification.xlsx
+++ b/back-end/uploadExcel/faculty_qualification.xlsx
@@ -753,15 +753,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="59.42578125" style="14" bestFit="1" customWidth="1"/>

</xml_diff>